<commit_message>
Represent number formats in pivot tables.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Other/PivotTableReferenceFiles/PivotTableWithNoneTheme/outputfile.xlsx
+++ b/ClosedXML.Tests/Resource/Other/PivotTableReferenceFiles/PivotTableWithNoneTheme/outputfile.xlsx
@@ -408,72 +408,72 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt2" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
-  <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <x:pivotFields count="6">
-    <x:pivotField name="Name" axis="axisRow" defaultSubtotal="0">
-      <x:items count="5">
-        <x:item x="0"/>
-        <x:item x="1"/>
-        <x:item x="2"/>
-        <x:item x="3"/>
-        <x:item x="4"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Code" defaultSubtotal="0"/>
-    <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
-    <x:pivotField name="Quality" defaultSubtotal="0"/>
-    <x:pivotField name="Month" axis="axisCol" defaultSubtotal="0">
-      <x:items count="1">
-        <x:item x="0"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="BakeDate" defaultSubtotal="0"/>
-  </x:pivotFields>
-  <x:rowFields count="1">
-    <x:field x="0"/>
-  </x:rowFields>
-  <x:rowItems count="6">
-    <x:i>
-      <x:x v="0"/>
-    </x:i>
-    <x:i>
-      <x:x v="1"/>
-    </x:i>
-    <x:i>
-      <x:x v="2"/>
-    </x:i>
-    <x:i>
-      <x:x v="3"/>
-    </x:i>
-    <x:i>
-      <x:x v="4"/>
-    </x:i>
-    <x:i t="grand">
-      <x:x/>
-    </x:i>
-  </x:rowItems>
-  <x:colFields count="1">
-    <x:field x="4"/>
-  </x:colFields>
-  <x:colItems count="2">
-    <x:i>
-      <x:x v="0"/>
-    </x:i>
-    <x:i t="grand">
-      <x:x/>
-    </x:i>
-  </x:colItems>
-  <x:dataFields count="1">
-    <x:dataField name="NumberOfOrdersPercentageOfBearclaw" fld="2" subtotal="sum" showDataAs="percent" baseField="0" baseItem="2" numFmtId="9"/>
-  </x:dataFields>
-  <x:pivotTableStyleInfo showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
-  <x:extLst>
-    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" enableEdit="0" hideValuesRow="1"/>
-    </x:ext>
-  </x:extLst>
-</x:pivotTableDefinition>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" updatedVersion="5">
+  <location ref="A1:C8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField name="Name" axis="axisRow" defaultSubtotal="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+      </items>
+    </pivotField>
+    <pivotField name="Code" defaultSubtotal="0"/>
+    <pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
+    <pivotField name="Quality" defaultSubtotal="0"/>
+    <pivotField name="Month" axis="axisCol" defaultSubtotal="0">
+      <items count="1">
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField name="BakeDate" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="4"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="NumberOfOrdersPercentageOfBearclaw" fld="2" showDataAs="percent" baseField="0" baseItem="2" numFmtId="9"/>
+  </dataFields>
+  <pivotTableStyleInfo showRowHeaders="1" showColHeaders="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition enableEdit="0" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>